<commit_message>
modified:   Jupyter scripts/main.ipynb 	modified:   Libaries/__pycache__/life_cycle_assessment.cpython-311.pyc 	modified:   Libaries/__pycache__/results_figures.cpython-311.pyc 	modified:   Libaries/life_cycle_assessment.py 	modified:   Libaries/results_figures.py 	modified:   data/database.xlsx 	modified:   data/temp.xlsx 	modified:   results/LCIA/LCIA_results.xlsx 	modified:   results/LCIA/LCIA_results_uniquie.xlsx 	modified:   results/figures/endpoint (H)_sc3.png 	modified:   results/figures/midpoint (H)_sc3.png
</commit_message>
<xml_diff>
--- a/data/database.xlsx
+++ b/data/database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruw\Desktop\RA\penicilin\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CCBD5C-FBBB-4DB4-92B7-454D05A9670D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25517ED0-A23C-4676-AC8E-B246A0FD83D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="37680" windowHeight="20580" xr2:uid="{8896788D-4D17-4058-8025-1A7424B43ED5}"/>
+    <workbookView xWindow="37320" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{8896788D-4D17-4058-8025-1A7424B43ED5}"/>
   </bookViews>
   <sheets>
     <sheet name="penicillin" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="214">
   <si>
     <t>Database</t>
   </si>
@@ -610,9 +610,6 @@
     <t>Scenerio2</t>
   </si>
   <si>
-    <t>vial sc3</t>
-  </si>
-  <si>
     <t>treatment of hazardous waste, hazardous waste incineration</t>
   </si>
   <si>
@@ -676,7 +673,10 @@
     <t>pill sc2</t>
   </si>
   <si>
-    <t>pill sc3</t>
+    <t>pill</t>
+  </si>
+  <si>
+    <t>combined sc3</t>
   </si>
 </sst>
 </file>
@@ -731,7 +731,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="26">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -875,12 +875,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -897,7 +891,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="318">
+  <cellXfs count="305">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -1246,21 +1240,6 @@
     <xf numFmtId="11" fontId="4" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="4" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="6" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="5" fillId="25" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="6" fillId="25" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="25" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="4" fillId="25" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="4" fillId="25" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="6" fillId="25" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
@@ -1487,10 +1466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE942774-4FA8-4DB9-ACB7-61C81F9E1DC2}">
-  <dimension ref="A1:I391"/>
+  <dimension ref="A1:I382"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A345" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C361" sqref="C361"/>
+    <sheetView tabSelected="1" topLeftCell="A214" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C344" sqref="C344"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1680,7 +1659,7 @@
         <v>18</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>23</v>
@@ -1706,7 +1685,7 @@
         <v>19</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>23</v>
@@ -1732,7 +1711,7 @@
         <v>20</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>23</v>
@@ -1758,7 +1737,7 @@
         <v>21</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>23</v>
@@ -1783,7 +1762,7 @@
         <v>22</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>24</v>
@@ -1847,7 +1826,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="25" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C20" s="21"/>
       <c r="D20" s="21"/>
@@ -1959,7 +1938,7 @@
         <v>18</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E25" s="23" t="s">
         <v>23</v>
@@ -1985,7 +1964,7 @@
         <v>20</v>
       </c>
       <c r="D26" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E26" s="23" t="s">
         <v>23</v>
@@ -2011,7 +1990,7 @@
         <v>34</v>
       </c>
       <c r="D27" s="23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E27" s="23" t="s">
         <v>23</v>
@@ -2037,7 +2016,7 @@
         <v>35</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E28" s="23" t="s">
         <v>23</v>
@@ -2063,7 +2042,7 @@
         <v>36</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E29" s="23" t="s">
         <v>23</v>
@@ -2088,7 +2067,7 @@
         <v>22</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E30" s="23" t="s">
         <v>24</v>
@@ -2113,7 +2092,7 @@
         <v>37</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E31" s="23" t="s">
         <v>24</v>
@@ -2177,7 +2156,7 @@
         <v>4</v>
       </c>
       <c r="B36" s="39" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C36" s="35"/>
       <c r="D36" s="35"/>
@@ -2288,7 +2267,7 @@
         <v>45</v>
       </c>
       <c r="D41" s="37" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E41" s="37" t="s">
         <v>23</v>
@@ -2313,7 +2292,7 @@
         <v>46</v>
       </c>
       <c r="D42" s="37" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E42" s="37" t="s">
         <v>23</v>
@@ -2338,7 +2317,7 @@
         <v>47</v>
       </c>
       <c r="D43" s="37" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E43" s="37" t="s">
         <v>23</v>
@@ -2363,7 +2342,7 @@
         <v>48</v>
       </c>
       <c r="D44" s="37" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E44" s="37" t="s">
         <v>23</v>
@@ -2388,7 +2367,7 @@
         <v>20</v>
       </c>
       <c r="D45" s="37" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E45" s="37" t="s">
         <v>23</v>
@@ -2413,7 +2392,7 @@
         <v>49</v>
       </c>
       <c r="D46" s="37" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E46" s="37" t="s">
         <v>23</v>
@@ -2438,7 +2417,7 @@
         <v>50</v>
       </c>
       <c r="D47" s="37" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E47" s="37" t="s">
         <v>23</v>
@@ -2463,7 +2442,7 @@
         <v>51</v>
       </c>
       <c r="D48" s="37" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E48" s="37" t="s">
         <v>23</v>
@@ -2488,7 +2467,7 @@
         <v>52</v>
       </c>
       <c r="D49" s="37" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E49" s="37" t="s">
         <v>23</v>
@@ -2513,7 +2492,7 @@
         <v>21</v>
       </c>
       <c r="D50" s="37" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E50" s="37" t="s">
         <v>23</v>
@@ -2538,7 +2517,7 @@
         <v>53</v>
       </c>
       <c r="D51" s="37" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E51" s="37" t="s">
         <v>23</v>
@@ -2602,7 +2581,7 @@
         <v>4</v>
       </c>
       <c r="B56" s="53" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C56" s="49"/>
       <c r="D56" s="49"/>
@@ -2713,7 +2692,7 @@
         <v>65</v>
       </c>
       <c r="D61" s="51" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E61" s="51" t="s">
         <v>23</v>
@@ -2738,7 +2717,7 @@
         <v>66</v>
       </c>
       <c r="D62" s="51" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E62" s="51" t="s">
         <v>23</v>
@@ -2802,7 +2781,7 @@
         <v>4</v>
       </c>
       <c r="B67" s="67" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C67" s="63"/>
       <c r="D67" s="63"/>
@@ -2913,7 +2892,7 @@
         <v>70</v>
       </c>
       <c r="D72" s="65" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E72" s="65" t="s">
         <v>23</v>
@@ -2938,7 +2917,7 @@
         <v>71</v>
       </c>
       <c r="D73" s="65" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E73" s="65" t="s">
         <v>23</v>
@@ -3002,7 +2981,7 @@
         <v>4</v>
       </c>
       <c r="B78" s="81" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C78" s="77"/>
       <c r="D78" s="77"/>
@@ -3113,7 +3092,7 @@
         <v>45</v>
       </c>
       <c r="D83" s="79" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E83" s="79" t="s">
         <v>23</v>
@@ -3138,7 +3117,7 @@
         <v>75</v>
       </c>
       <c r="D84" s="79" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E84" s="79" t="s">
         <v>23</v>
@@ -3163,7 +3142,7 @@
         <v>47</v>
       </c>
       <c r="D85" s="79" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E85" s="79" t="s">
         <v>23</v>
@@ -3188,7 +3167,7 @@
         <v>49</v>
       </c>
       <c r="D86" s="79" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E86" s="79" t="s">
         <v>23</v>
@@ -3213,7 +3192,7 @@
         <v>50</v>
       </c>
       <c r="D87" s="79" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E87" s="79" t="s">
         <v>23</v>
@@ -3238,7 +3217,7 @@
         <v>35</v>
       </c>
       <c r="D88" s="79" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E88" s="79" t="s">
         <v>23</v>
@@ -3257,7 +3236,7 @@
         <v>1</v>
       </c>
       <c r="B90" s="90" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C90" s="91"/>
       <c r="D90" s="92"/>
@@ -3302,7 +3281,7 @@
         <v>4</v>
       </c>
       <c r="B93" s="95" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C93" s="91"/>
       <c r="D93" s="91"/>
@@ -3413,7 +3392,7 @@
         <v>78</v>
       </c>
       <c r="D98" s="93" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E98" s="93" t="s">
         <v>23</v>
@@ -3438,7 +3417,7 @@
         <v>79</v>
       </c>
       <c r="D99" s="93" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E99" s="93" t="s">
         <v>84</v>
@@ -3463,7 +3442,7 @@
         <v>80</v>
       </c>
       <c r="D100" s="93" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E100" s="93" t="s">
         <v>23</v>
@@ -3488,7 +3467,7 @@
         <v>81</v>
       </c>
       <c r="D101" s="93" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E101" s="93" t="s">
         <v>23</v>
@@ -3513,7 +3492,7 @@
         <v>52</v>
       </c>
       <c r="D102" s="93" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E102" s="93" t="s">
         <v>23</v>
@@ -3568,7 +3547,7 @@
         <v>82</v>
       </c>
       <c r="D104" s="93" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E104" s="93" t="s">
         <v>24</v>
@@ -3593,7 +3572,7 @@
         <v>83</v>
       </c>
       <c r="D105" s="93" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E105" s="93" t="s">
         <v>24</v>
@@ -3612,7 +3591,7 @@
         <v>1</v>
       </c>
       <c r="B107" s="104" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C107" s="105"/>
       <c r="D107" s="106"/>
@@ -3657,7 +3636,7 @@
         <v>4</v>
       </c>
       <c r="B110" s="109" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C110" s="105"/>
       <c r="D110" s="105"/>
@@ -3768,7 +3747,7 @@
         <v>92</v>
       </c>
       <c r="D115" s="107" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E115" s="107" t="s">
         <v>23</v>
@@ -3793,7 +3772,7 @@
         <v>93</v>
       </c>
       <c r="D116" s="107" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E116" s="107" t="s">
         <v>23</v>
@@ -3818,7 +3797,7 @@
         <v>94</v>
       </c>
       <c r="D117" s="107" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E117" s="107" t="s">
         <v>23</v>
@@ -3844,7 +3823,7 @@
         <v>79</v>
       </c>
       <c r="D118" s="107" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E118" s="107" t="s">
         <v>84</v>
@@ -3869,7 +3848,7 @@
         <v>95</v>
       </c>
       <c r="D119" s="107" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E119" s="107" t="s">
         <v>23</v>
@@ -3894,7 +3873,7 @@
         <v>96</v>
       </c>
       <c r="D120" s="107" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E120" s="107" t="s">
         <v>148</v>
@@ -3919,7 +3898,7 @@
         <v>97</v>
       </c>
       <c r="D121" s="107" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E121" s="107" t="s">
         <v>23</v>
@@ -3974,7 +3953,7 @@
         <v>98</v>
       </c>
       <c r="D123" s="107" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E123" s="107" t="s">
         <v>23</v>
@@ -4030,7 +4009,7 @@
         <v>99</v>
       </c>
       <c r="D125" s="107" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E125" s="107" t="s">
         <v>23</v>
@@ -4055,7 +4034,7 @@
         <v>100</v>
       </c>
       <c r="D126" s="107" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E126" s="107" t="s">
         <v>23</v>
@@ -4080,7 +4059,7 @@
         <v>101</v>
       </c>
       <c r="D127" s="107" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E127" s="107" t="s">
         <v>23</v>
@@ -4105,7 +4084,7 @@
         <v>115</v>
       </c>
       <c r="D128" s="107" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E128" s="107" t="s">
         <v>23</v>
@@ -4130,7 +4109,7 @@
         <v>116</v>
       </c>
       <c r="D129" s="107" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E129" s="107" t="s">
         <v>23</v>
@@ -4245,7 +4224,7 @@
     </row>
     <row r="134" spans="1:9">
       <c r="A134" s="107" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B134" s="107">
         <v>6.58</v>
@@ -4359,7 +4338,7 @@
       <c r="I138" s="107"/>
     </row>
     <row r="139" spans="1:9">
-      <c r="B139" s="317"/>
+      <c r="B139" s="304"/>
     </row>
     <row r="140" spans="1:9" ht="15.75">
       <c r="A140" s="117" t="s">
@@ -4411,7 +4390,7 @@
         <v>4</v>
       </c>
       <c r="B143" s="123" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C143" s="119"/>
       <c r="D143" s="119"/>
@@ -4520,7 +4499,7 @@
         <v>128</v>
       </c>
       <c r="D148" s="121" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E148" s="121" t="s">
         <v>23</v>
@@ -4545,7 +4524,7 @@
         <v>129</v>
       </c>
       <c r="D149" s="121" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E149" s="121" t="s">
         <v>23</v>
@@ -4570,7 +4549,7 @@
         <v>130</v>
       </c>
       <c r="D150" s="121" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E150" s="121" t="s">
         <v>23</v>
@@ -4595,7 +4574,7 @@
         <v>131</v>
       </c>
       <c r="D151" s="121" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E151" s="121" t="s">
         <v>23</v>
@@ -4620,7 +4599,7 @@
         <v>101</v>
       </c>
       <c r="D152" s="121" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E152" s="121" t="s">
         <v>23</v>
@@ -4645,7 +4624,7 @@
         <v>132</v>
       </c>
       <c r="D153" s="121" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E153" s="121" t="s">
         <v>23</v>
@@ -4709,7 +4688,7 @@
         <v>4</v>
       </c>
       <c r="B158" s="137" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C158" s="133"/>
       <c r="D158" s="133"/>
@@ -4820,7 +4799,7 @@
         <v>92</v>
       </c>
       <c r="D163" s="135" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E163" s="135" t="s">
         <v>23</v>
@@ -4845,7 +4824,7 @@
         <v>93</v>
       </c>
       <c r="D164" s="135" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E164" s="135" t="s">
         <v>23</v>
@@ -4870,7 +4849,7 @@
         <v>94</v>
       </c>
       <c r="D165" s="135" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E165" s="135" t="s">
         <v>23</v>
@@ -4896,7 +4875,7 @@
         <v>79</v>
       </c>
       <c r="D166" s="135" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E166" s="135" t="s">
         <v>84</v>
@@ -4921,7 +4900,7 @@
         <v>95</v>
       </c>
       <c r="D167" s="135" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E167" s="135" t="s">
         <v>23</v>
@@ -4946,7 +4925,7 @@
         <v>139</v>
       </c>
       <c r="D168" s="135" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E168" s="135" t="s">
         <v>148</v>
@@ -4971,7 +4950,7 @@
         <v>97</v>
       </c>
       <c r="D169" s="135" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E169" s="135" t="s">
         <v>23</v>
@@ -5026,7 +5005,7 @@
         <v>140</v>
       </c>
       <c r="D171" s="135" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E171" s="135" t="s">
         <v>23</v>
@@ -5081,7 +5060,7 @@
         <v>99</v>
       </c>
       <c r="D173" s="135" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E173" s="135" t="s">
         <v>23</v>
@@ -5106,7 +5085,7 @@
         <v>100</v>
       </c>
       <c r="D174" s="135" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E174" s="135" t="s">
         <v>23</v>
@@ -5131,7 +5110,7 @@
         <v>101</v>
       </c>
       <c r="D175" s="135" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E175" s="135" t="s">
         <v>23</v>
@@ -5156,7 +5135,7 @@
         <v>115</v>
       </c>
       <c r="D176" s="135" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E176" s="135" t="s">
         <v>23</v>
@@ -5181,7 +5160,7 @@
         <v>116</v>
       </c>
       <c r="D177" s="135" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E177" s="135" t="s">
         <v>23</v>
@@ -5296,7 +5275,7 @@
     </row>
     <row r="182" spans="1:9">
       <c r="A182" s="135" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B182" s="135">
         <v>6.58</v>
@@ -5459,7 +5438,7 @@
         <v>4</v>
       </c>
       <c r="B191" s="151" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C191" s="147"/>
       <c r="D191" s="147"/>
@@ -5570,7 +5549,7 @@
         <v>78</v>
       </c>
       <c r="D196" s="149" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E196" s="149" t="s">
         <v>23</v>
@@ -5595,7 +5574,7 @@
         <v>151</v>
       </c>
       <c r="D197" s="149" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E197" s="149" t="s">
         <v>23</v>
@@ -5620,7 +5599,7 @@
         <v>22</v>
       </c>
       <c r="D198" s="149" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E198" s="149" t="s">
         <v>24</v>
@@ -5645,7 +5624,7 @@
         <v>152</v>
       </c>
       <c r="D199" s="149" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E199" s="149" t="s">
         <v>24</v>
@@ -5701,7 +5680,7 @@
         <v>116</v>
       </c>
       <c r="D201" s="149" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E201" s="149" t="s">
         <v>23</v>
@@ -5727,7 +5706,7 @@
         <v>155</v>
       </c>
       <c r="D202" s="149" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E202" s="149" t="s">
         <v>23</v>
@@ -5746,7 +5725,7 @@
         <v>1</v>
       </c>
       <c r="B204" s="160" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C204" s="161"/>
       <c r="D204" s="162"/>
@@ -5776,7 +5755,7 @@
         <v>3</v>
       </c>
       <c r="B206" s="166" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C206" s="161"/>
       <c r="D206" s="161"/>
@@ -5791,7 +5770,7 @@
         <v>4</v>
       </c>
       <c r="B207" s="165" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C207" s="161"/>
       <c r="D207" s="161"/>
@@ -5902,7 +5881,7 @@
         <v>78</v>
       </c>
       <c r="D212" s="163" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E212" s="163" t="s">
         <v>23</v>
@@ -5927,7 +5906,7 @@
         <v>151</v>
       </c>
       <c r="D213" s="163" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E213" s="163" t="s">
         <v>23</v>
@@ -5982,7 +5961,7 @@
         <v>157</v>
       </c>
       <c r="D215" s="163" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E215" s="163" t="s">
         <v>23</v>
@@ -6007,7 +5986,7 @@
         <v>22</v>
       </c>
       <c r="D216" s="163" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E216" s="163" t="s">
         <v>24</v>
@@ -6033,7 +6012,7 @@
         <v>159</v>
       </c>
       <c r="D217" s="163" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E217" s="163" t="s">
         <v>23</v>
@@ -6052,7 +6031,7 @@
         <v>1</v>
       </c>
       <c r="B219" s="174" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C219" s="175"/>
       <c r="D219" s="176"/>
@@ -6082,7 +6061,7 @@
         <v>3</v>
       </c>
       <c r="B221" s="180" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C221" s="175"/>
       <c r="D221" s="175"/>
@@ -6097,7 +6076,7 @@
         <v>4</v>
       </c>
       <c r="B222" s="179" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C222" s="175"/>
       <c r="D222" s="175"/>
@@ -6208,7 +6187,7 @@
         <v>75</v>
       </c>
       <c r="D227" s="177" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E227" s="177" t="s">
         <v>23</v>
@@ -6233,7 +6212,7 @@
         <v>79</v>
       </c>
       <c r="D228" s="177" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E228" s="177" t="s">
         <v>84</v>
@@ -6258,7 +6237,7 @@
         <v>46</v>
       </c>
       <c r="D229" s="177" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E229" s="177" t="s">
         <v>23</v>
@@ -6283,7 +6262,7 @@
         <v>161</v>
       </c>
       <c r="D230" s="177" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E230" s="177" t="s">
         <v>23</v>
@@ -6308,7 +6287,7 @@
         <v>162</v>
       </c>
       <c r="D231" s="177" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E231" s="177" t="s">
         <v>23</v>
@@ -6333,7 +6312,7 @@
         <v>47</v>
       </c>
       <c r="D232" s="177" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E232" s="177" t="s">
         <v>23</v>
@@ -6358,7 +6337,7 @@
         <v>50</v>
       </c>
       <c r="D233" s="177" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E233" s="177" t="s">
         <v>23</v>
@@ -6413,7 +6392,7 @@
         <v>35</v>
       </c>
       <c r="D235" s="177" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E235" s="177" t="s">
         <v>23</v>
@@ -6438,7 +6417,7 @@
         <v>163</v>
       </c>
       <c r="D236" s="177" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E236" s="177" t="s">
         <v>24</v>
@@ -6463,7 +6442,7 @@
         <v>83</v>
       </c>
       <c r="D237" s="177" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E237" s="177" t="s">
         <v>24</v>
@@ -6527,7 +6506,7 @@
         <v>4</v>
       </c>
       <c r="B242" s="193" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C242" s="189"/>
       <c r="D242" s="189"/>
@@ -6638,7 +6617,7 @@
         <v>169</v>
       </c>
       <c r="D247" s="191" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E247" s="191" t="s">
         <v>23</v>
@@ -6663,7 +6642,7 @@
         <v>99</v>
       </c>
       <c r="D248" s="191" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E248" s="191" t="s">
         <v>23</v>
@@ -6727,7 +6706,7 @@
         <v>4</v>
       </c>
       <c r="B253" s="206" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C253" s="202"/>
       <c r="D253" s="202"/>
@@ -6838,7 +6817,7 @@
         <v>47</v>
       </c>
       <c r="D258" s="204" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E258" s="204" t="s">
         <v>23</v>
@@ -6863,7 +6842,7 @@
         <v>49</v>
       </c>
       <c r="D259" s="204" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E259" s="204" t="s">
         <v>23</v>
@@ -6888,7 +6867,7 @@
         <v>34</v>
       </c>
       <c r="D260" s="204" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E260" s="204" t="s">
         <v>23</v>
@@ -6952,7 +6931,7 @@
         <v>4</v>
       </c>
       <c r="B265" s="219" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C265" s="215"/>
       <c r="D265" s="215"/>
@@ -7063,7 +7042,7 @@
         <v>173</v>
       </c>
       <c r="D270" s="217" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E270" s="217" t="s">
         <v>23</v>
@@ -7088,7 +7067,7 @@
         <v>79</v>
       </c>
       <c r="D271" s="217" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E271" s="217" t="s">
         <v>84</v>
@@ -7113,7 +7092,7 @@
         <v>65</v>
       </c>
       <c r="D272" s="217" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E272" s="217" t="s">
         <v>23</v>
@@ -7228,7 +7207,7 @@
         <v>174</v>
       </c>
       <c r="D276" s="217" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E276" s="217" t="s">
         <v>23</v>
@@ -7253,7 +7232,7 @@
         <v>175</v>
       </c>
       <c r="D277" s="217" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E277" s="217" t="s">
         <v>23</v>
@@ -7278,7 +7257,7 @@
         <v>176</v>
       </c>
       <c r="D278" s="217" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E278" s="217" t="s">
         <v>23</v>
@@ -7603,7 +7582,7 @@
         <v>184</v>
       </c>
       <c r="D293" s="230" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E293" s="230" t="s">
         <v>23</v>
@@ -7659,7 +7638,7 @@
         <v>176</v>
       </c>
       <c r="D295" s="230" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E295" s="230" t="s">
         <v>23</v>
@@ -7925,7 +7904,7 @@
         <v>181</v>
       </c>
       <c r="D308" s="243" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E308" s="243" t="s">
         <v>23</v>
@@ -8011,7 +7990,7 @@
         <v>184</v>
       </c>
       <c r="D311" s="243" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E311" s="243" t="s">
         <v>23</v>
@@ -8067,7 +8046,7 @@
         <v>176</v>
       </c>
       <c r="D313" s="243" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E313" s="243" t="s">
         <v>23</v>
@@ -8093,7 +8072,7 @@
         <v>159</v>
       </c>
       <c r="D314" s="243" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E314" s="243" t="s">
         <v>23</v>
@@ -8383,7 +8362,7 @@
         <v>181</v>
       </c>
       <c r="D328" s="256" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E328" s="256" t="s">
         <v>23</v>
@@ -8469,7 +8448,7 @@
         <v>184</v>
       </c>
       <c r="D331" s="256" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E331" s="256" t="s">
         <v>23</v>
@@ -8524,7 +8503,7 @@
         <v>176</v>
       </c>
       <c r="D333" s="256" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E333" s="256" t="s">
         <v>23</v>
@@ -8550,7 +8529,7 @@
         <v>159</v>
       </c>
       <c r="D334" s="256" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E334" s="256" t="s">
         <v>23</v>
@@ -8593,7 +8572,7 @@
         <v>1</v>
       </c>
       <c r="B337" s="266" t="s">
-        <v>191</v>
+        <v>213</v>
       </c>
       <c r="C337" s="267"/>
       <c r="D337" s="268"/>
@@ -8623,7 +8602,7 @@
         <v>3</v>
       </c>
       <c r="B339" s="272" t="s">
-        <v>191</v>
+        <v>213</v>
       </c>
       <c r="C339" s="267"/>
       <c r="D339" s="267"/>
@@ -8708,7 +8687,7 @@
     <row r="344" spans="1:9">
       <c r="A344" s="275" t="str">
         <f>B337</f>
-        <v>vial sc3</v>
+        <v>combined sc3</v>
       </c>
       <c r="B344" s="276">
         <f>B338</f>
@@ -8716,7 +8695,7 @@
       </c>
       <c r="C344" s="275" t="str">
         <f>B339</f>
-        <v>vial sc3</v>
+        <v>combined sc3</v>
       </c>
       <c r="D344" s="275" t="str">
         <f>B340</f>
@@ -8735,7 +8714,7 @@
         <v>penicillin</v>
       </c>
       <c r="I344" s="269" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="345" spans="1:9">
@@ -8766,7 +8745,9 @@
         <f t="shared" ref="H345" si="28">H$10</f>
         <v>penicillin</v>
       </c>
-      <c r="I345" s="269"/>
+      <c r="I345" s="269" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="346" spans="1:9">
       <c r="A346" s="275" t="str">
@@ -8796,7 +8777,9 @@
         <f t="shared" ref="H346" si="30">H$195</f>
         <v>penicillin</v>
       </c>
-      <c r="I346" s="269"/>
+      <c r="I346" s="269" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="347" spans="1:9">
       <c r="A347" s="275" t="str">
@@ -8826,7 +8809,9 @@
         <f t="shared" ref="H347" si="32">H$24</f>
         <v>penicillin</v>
       </c>
-      <c r="I347" s="269"/>
+      <c r="I347" s="269" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="348" spans="1:9">
       <c r="A348" s="269" t="s">
@@ -8840,7 +8825,7 @@
         <v>181</v>
       </c>
       <c r="D348" s="269" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E348" s="269" t="s">
         <v>23</v>
@@ -8852,7 +8837,9 @@
       <c r="H348" s="269" t="s">
         <v>17</v>
       </c>
-      <c r="I348" s="269"/>
+      <c r="I348" s="269" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="349" spans="1:9">
       <c r="A349" s="275" t="str">
@@ -8882,7 +8869,9 @@
         <f t="shared" ref="H349" si="34">H$40</f>
         <v>penicillin</v>
       </c>
-      <c r="I349" s="269"/>
+      <c r="I349" s="269" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="350" spans="1:9">
       <c r="A350" s="275" t="str">
@@ -8912,7 +8901,9 @@
         <f t="shared" ref="H350" si="36">H$82</f>
         <v>penicillin</v>
       </c>
-      <c r="I350" s="269"/>
+      <c r="I350" s="269" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="351" spans="1:9">
       <c r="A351" s="269" t="s">
@@ -8926,7 +8917,7 @@
         <v>184</v>
       </c>
       <c r="D351" s="269" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E351" s="269" t="s">
         <v>23</v>
@@ -8938,7 +8929,9 @@
       <c r="H351" s="269" t="s">
         <v>17</v>
       </c>
-      <c r="I351" s="269"/>
+      <c r="I351" s="269" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="352" spans="1:9">
       <c r="A352" s="275" t="str">
@@ -8968,7 +8961,9 @@
         <f t="shared" ref="H352" si="38">H$257</f>
         <v>penicillin</v>
       </c>
-      <c r="I352" s="269"/>
+      <c r="I352" s="269" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="353" spans="1:9">
       <c r="A353" s="269" t="s">
@@ -8982,7 +8977,7 @@
         <v>176</v>
       </c>
       <c r="D353" s="269" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E353" s="269" t="s">
         <v>23</v>
@@ -8994,7 +8989,9 @@
       <c r="H353" s="269" t="s">
         <v>17</v>
       </c>
-      <c r="I353" s="269"/>
+      <c r="I353" s="269" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="354" spans="1:9">
       <c r="A354" s="269" t="s">
@@ -9008,7 +9005,7 @@
         <v>159</v>
       </c>
       <c r="D354" s="269" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E354" s="269" t="s">
         <v>23</v>
@@ -9020,7 +9017,9 @@
       <c r="H354" s="269" t="s">
         <v>17</v>
       </c>
-      <c r="I354" s="269"/>
+      <c r="I354" s="269" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="355" spans="1:9">
       <c r="A355" s="269" t="s">
@@ -9044,62 +9043,108 @@
       <c r="H355" s="269" t="s">
         <v>125</v>
       </c>
-      <c r="I355" s="269"/>
-    </row>
-    <row r="357" spans="1:9" ht="15.75">
-      <c r="A357" s="278" t="s">
+      <c r="I355" s="269" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="356" spans="1:9">
+      <c r="A356" s="269" t="s">
+        <v>191</v>
+      </c>
+      <c r="B356" s="275">
+        <f>3.564*10^-3</f>
+        <v>3.5640000000000003E-3</v>
+      </c>
+      <c r="C356" s="269" t="s">
+        <v>181</v>
+      </c>
+      <c r="D356" s="269" t="s">
+        <v>202</v>
+      </c>
+      <c r="E356" s="269" t="s">
+        <v>23</v>
+      </c>
+      <c r="F356" s="269"/>
+      <c r="G356" s="269" t="s">
+        <v>25</v>
+      </c>
+      <c r="H356" s="269" t="s">
+        <v>17</v>
+      </c>
+      <c r="I356" s="269" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="357" spans="1:9">
+      <c r="A357" s="269" t="str">
+        <f>A211</f>
+        <v>packed box of penicillin</v>
+      </c>
+      <c r="B357" s="275">
+        <f>4/10</f>
+        <v>0.4</v>
+      </c>
+      <c r="C357" s="269" t="str">
+        <f>C211</f>
+        <v>box of penicillin</v>
+      </c>
+      <c r="D357" s="269" t="str">
+        <f>D211</f>
+        <v>SE</v>
+      </c>
+      <c r="E357" s="269" t="str">
+        <f>E211</f>
+        <v>unit</v>
+      </c>
+      <c r="F357" s="269"/>
+      <c r="G357" s="269" t="s">
+        <v>25</v>
+      </c>
+      <c r="H357" s="269" t="str">
+        <f>H211</f>
+        <v>penicillin</v>
+      </c>
+      <c r="I357" s="269" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="358" spans="1:9">
+      <c r="A358" s="269" t="s">
+        <v>160</v>
+      </c>
+      <c r="B358" s="275">
+        <f>-31.584*10^-3</f>
+        <v>-3.1584000000000001E-2</v>
+      </c>
+      <c r="C358" s="269" t="s">
+        <v>159</v>
+      </c>
+      <c r="D358" s="269" t="s">
+        <v>202</v>
+      </c>
+      <c r="E358" s="269" t="s">
+        <v>23</v>
+      </c>
+      <c r="F358" s="269"/>
+      <c r="G358" s="269" t="s">
+        <v>25</v>
+      </c>
+      <c r="H358" s="269" t="s">
+        <v>17</v>
+      </c>
+      <c r="I358" s="269" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="360" spans="1:9" ht="15.75">
+      <c r="A360" s="278" t="s">
         <v>1</v>
       </c>
-      <c r="B357" s="279" t="s">
-        <v>211</v>
-      </c>
-      <c r="C357" s="280"/>
-      <c r="D357" s="281"/>
-      <c r="E357" s="280"/>
-      <c r="F357" s="282"/>
-      <c r="G357" s="280"/>
-      <c r="H357" s="280"/>
-      <c r="I357" s="280"/>
-    </row>
-    <row r="358" spans="1:9">
-      <c r="A358" s="283" t="s">
-        <v>2</v>
-      </c>
-      <c r="B358" s="284">
-        <v>1</v>
-      </c>
-      <c r="C358" s="280"/>
-      <c r="D358" s="280"/>
-      <c r="E358" s="280"/>
-      <c r="F358" s="282"/>
-      <c r="G358" s="280"/>
-      <c r="H358" s="280"/>
-      <c r="I358" s="280"/>
-    </row>
-    <row r="359" spans="1:9">
-      <c r="A359" s="283" t="s">
-        <v>3</v>
-      </c>
-      <c r="B359" s="285" t="s">
-        <v>211</v>
-      </c>
-      <c r="C359" s="280"/>
-      <c r="D359" s="280"/>
-      <c r="E359" s="280"/>
-      <c r="F359" s="282"/>
-      <c r="G359" s="280"/>
-      <c r="H359" s="280"/>
-      <c r="I359" s="280"/>
-    </row>
-    <row r="360" spans="1:9">
-      <c r="A360" s="283" t="s">
-        <v>4</v>
-      </c>
-      <c r="B360" s="284" t="s">
-        <v>31</v>
+      <c r="B360" s="279" t="s">
+        <v>210</v>
       </c>
       <c r="C360" s="280"/>
-      <c r="D360" s="280"/>
+      <c r="D360" s="281"/>
       <c r="E360" s="280"/>
       <c r="F360" s="282"/>
       <c r="G360" s="280"/>
@@ -9108,10 +9153,10 @@
     </row>
     <row r="361" spans="1:9">
       <c r="A361" s="283" t="s">
-        <v>5</v>
-      </c>
-      <c r="B361" s="285" t="s">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="B361" s="284">
+        <v>1</v>
       </c>
       <c r="C361" s="280"/>
       <c r="D361" s="280"/>
@@ -9121,217 +9166,217 @@
       <c r="H361" s="280"/>
       <c r="I361" s="280"/>
     </row>
-    <row r="362" spans="1:9" ht="15.75">
-      <c r="A362" s="286" t="s">
+    <row r="362" spans="1:9">
+      <c r="A362" s="283" t="s">
+        <v>3</v>
+      </c>
+      <c r="B362" s="285" t="s">
+        <v>210</v>
+      </c>
+      <c r="C362" s="280"/>
+      <c r="D362" s="280"/>
+      <c r="E362" s="280"/>
+      <c r="F362" s="282"/>
+      <c r="G362" s="280"/>
+      <c r="H362" s="280"/>
+      <c r="I362" s="280"/>
+    </row>
+    <row r="363" spans="1:9">
+      <c r="A363" s="283" t="s">
+        <v>4</v>
+      </c>
+      <c r="B363" s="284" t="s">
+        <v>31</v>
+      </c>
+      <c r="C363" s="280"/>
+      <c r="D363" s="280"/>
+      <c r="E363" s="280"/>
+      <c r="F363" s="282"/>
+      <c r="G363" s="280"/>
+      <c r="H363" s="280"/>
+      <c r="I363" s="280"/>
+    </row>
+    <row r="364" spans="1:9">
+      <c r="A364" s="283" t="s">
+        <v>5</v>
+      </c>
+      <c r="B364" s="285" t="s">
+        <v>5</v>
+      </c>
+      <c r="C364" s="280"/>
+      <c r="D364" s="280"/>
+      <c r="E364" s="280"/>
+      <c r="F364" s="282"/>
+      <c r="G364" s="280"/>
+      <c r="H364" s="280"/>
+      <c r="I364" s="280"/>
+    </row>
+    <row r="365" spans="1:9" ht="15.75">
+      <c r="A365" s="286" t="s">
         <v>6</v>
       </c>
-      <c r="B362" s="279"/>
-      <c r="C362" s="286"/>
-      <c r="D362" s="286"/>
-      <c r="E362" s="286"/>
-      <c r="F362" s="282"/>
-      <c r="G362" s="286"/>
-      <c r="H362" s="286"/>
-      <c r="I362" s="286"/>
-    </row>
-    <row r="363" spans="1:9" ht="15.75">
-      <c r="A363" s="286" t="s">
+      <c r="B365" s="279"/>
+      <c r="C365" s="286"/>
+      <c r="D365" s="286"/>
+      <c r="E365" s="286"/>
+      <c r="F365" s="282"/>
+      <c r="G365" s="286"/>
+      <c r="H365" s="286"/>
+      <c r="I365" s="286"/>
+    </row>
+    <row r="366" spans="1:9" ht="15.75">
+      <c r="A366" s="286" t="s">
         <v>7</v>
       </c>
-      <c r="B363" s="279" t="s">
+      <c r="B366" s="279" t="s">
         <v>8</v>
       </c>
-      <c r="C363" s="286" t="s">
+      <c r="C366" s="286" t="s">
         <v>3</v>
       </c>
-      <c r="D363" s="286" t="s">
+      <c r="D366" s="286" t="s">
         <v>4</v>
       </c>
-      <c r="E363" s="286" t="s">
+      <c r="E366" s="286" t="s">
         <v>5</v>
       </c>
-      <c r="F363" s="287" t="s">
+      <c r="F366" s="287" t="s">
         <v>9</v>
       </c>
-      <c r="G363" s="286" t="s">
+      <c r="G366" s="286" t="s">
         <v>10</v>
       </c>
-      <c r="H363" s="286" t="s">
+      <c r="H366" s="286" t="s">
         <v>11</v>
       </c>
-      <c r="I363" s="286" t="s">
+      <c r="I366" s="286" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="364" spans="1:9">
-      <c r="A364" s="288" t="str">
-        <f>B357</f>
+    <row r="367" spans="1:9">
+      <c r="A367" s="288" t="str">
+        <f>B360</f>
         <v>pill sc1</v>
       </c>
-      <c r="B364" s="289">
-        <f>B358</f>
+      <c r="B367" s="289">
+        <f>B361</f>
         <v>1</v>
       </c>
-      <c r="C364" s="288" t="str">
-        <f>B359</f>
+      <c r="C367" s="288" t="str">
+        <f>B362</f>
         <v>pill sc1</v>
       </c>
-      <c r="D364" s="288" t="str">
-        <f>B360</f>
+      <c r="D367" s="288" t="str">
+        <f>B363</f>
         <v>DK</v>
       </c>
-      <c r="E364" s="288" t="str">
-        <f>B361</f>
+      <c r="E367" s="288" t="str">
+        <f>B364</f>
         <v>unit</v>
       </c>
-      <c r="F364" s="282"/>
-      <c r="G364" s="282" t="s">
+      <c r="F367" s="282"/>
+      <c r="G367" s="282" t="s">
         <v>13</v>
       </c>
-      <c r="H364" s="290" t="str">
+      <c r="H367" s="290" t="str">
         <f>$B$1</f>
         <v>penicillin</v>
       </c>
-      <c r="I364" s="282" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="365" spans="1:9">
-      <c r="A365" s="282" t="s">
+      <c r="I367" s="282" t="s">
         <v>192</v>
       </c>
-      <c r="B365" s="288">
+    </row>
+    <row r="368" spans="1:9">
+      <c r="A368" s="282" t="s">
+        <v>191</v>
+      </c>
+      <c r="B368" s="288">
         <f>0.297*10^-3</f>
         <v>2.9700000000000001E-4</v>
       </c>
-      <c r="C365" s="282" t="s">
+      <c r="C368" s="282" t="s">
         <v>181</v>
       </c>
-      <c r="D365" s="282" t="s">
-        <v>203</v>
-      </c>
-      <c r="E365" s="282" t="s">
-        <v>23</v>
-      </c>
-      <c r="F365" s="282"/>
-      <c r="G365" s="282" t="s">
-        <v>25</v>
-      </c>
-      <c r="H365" s="282" t="s">
-        <v>17</v>
-      </c>
-      <c r="I365" s="282"/>
-    </row>
-    <row r="366" spans="1:9">
-      <c r="A366" s="288" t="str">
+      <c r="D368" s="282" t="s">
+        <v>202</v>
+      </c>
+      <c r="E368" s="282" t="s">
+        <v>23</v>
+      </c>
+      <c r="F368" s="282"/>
+      <c r="G368" s="282" t="s">
+        <v>25</v>
+      </c>
+      <c r="H368" s="282" t="s">
+        <v>17</v>
+      </c>
+      <c r="I368" s="282"/>
+    </row>
+    <row r="369" spans="1:9">
+      <c r="A369" s="288" t="str">
         <f>A211</f>
         <v>packed box of penicillin</v>
       </c>
-      <c r="B366" s="289">
+      <c r="B369" s="289">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="C366" s="288" t="str">
+      <c r="C369" s="288" t="str">
         <f>C211</f>
         <v>box of penicillin</v>
       </c>
-      <c r="D366" s="288" t="str">
-        <f t="shared" ref="D366:E366" si="39">D211</f>
+      <c r="D369" s="288" t="str">
+        <f t="shared" ref="D369:E369" si="39">D211</f>
         <v>SE</v>
       </c>
-      <c r="E366" s="288" t="str">
+      <c r="E369" s="288" t="str">
         <f t="shared" si="39"/>
         <v>unit</v>
       </c>
-      <c r="F366" s="282"/>
-      <c r="G366" s="282" t="s">
-        <v>25</v>
-      </c>
-      <c r="H366" s="288" t="str">
-        <f t="shared" ref="H366" si="40">H211</f>
+      <c r="F369" s="282"/>
+      <c r="G369" s="282" t="s">
+        <v>25</v>
+      </c>
+      <c r="H369" s="288" t="str">
+        <f t="shared" ref="H369" si="40">H211</f>
         <v>penicillin</v>
       </c>
-      <c r="I366" s="282"/>
-    </row>
-    <row r="367" spans="1:9">
-      <c r="A367" s="282" t="s">
+      <c r="I369" s="282"/>
+    </row>
+    <row r="370" spans="1:9">
+      <c r="A370" s="282" t="s">
         <v>160</v>
       </c>
-      <c r="B367" s="288">
+      <c r="B370" s="288">
         <f>-2.632*10^-3</f>
         <v>-2.6320000000000002E-3</v>
       </c>
-      <c r="C367" s="282" t="s">
+      <c r="C370" s="282" t="s">
         <v>159</v>
       </c>
-      <c r="D367" s="282" t="s">
-        <v>203</v>
-      </c>
-      <c r="E367" s="282" t="s">
-        <v>23</v>
-      </c>
-      <c r="F367" s="282"/>
-      <c r="G367" s="282" t="s">
-        <v>25</v>
-      </c>
-      <c r="H367" s="282" t="s">
-        <v>17</v>
-      </c>
-      <c r="I367" s="282"/>
-    </row>
-    <row r="369" spans="1:9" ht="15.75">
-      <c r="A369" s="291" t="s">
+      <c r="D370" s="282" t="s">
+        <v>202</v>
+      </c>
+      <c r="E370" s="282" t="s">
+        <v>23</v>
+      </c>
+      <c r="F370" s="282"/>
+      <c r="G370" s="282" t="s">
+        <v>25</v>
+      </c>
+      <c r="H370" s="282" t="s">
+        <v>17</v>
+      </c>
+      <c r="I370" s="282"/>
+    </row>
+    <row r="372" spans="1:9" ht="15.75">
+      <c r="A372" s="291" t="s">
         <v>1</v>
       </c>
-      <c r="B369" s="292" t="s">
-        <v>212</v>
-      </c>
-      <c r="C369" s="293"/>
-      <c r="D369" s="294"/>
-      <c r="E369" s="293"/>
-      <c r="F369" s="295"/>
-      <c r="G369" s="293"/>
-      <c r="H369" s="293"/>
-      <c r="I369" s="293"/>
-    </row>
-    <row r="370" spans="1:9">
-      <c r="A370" s="296" t="s">
-        <v>2</v>
-      </c>
-      <c r="B370" s="297">
-        <v>1</v>
-      </c>
-      <c r="C370" s="293"/>
-      <c r="D370" s="293"/>
-      <c r="E370" s="293"/>
-      <c r="F370" s="295"/>
-      <c r="G370" s="293"/>
-      <c r="H370" s="293"/>
-      <c r="I370" s="293"/>
-    </row>
-    <row r="371" spans="1:9">
-      <c r="A371" s="296" t="s">
-        <v>3</v>
-      </c>
-      <c r="B371" s="298" t="s">
-        <v>212</v>
-      </c>
-      <c r="C371" s="293"/>
-      <c r="D371" s="293"/>
-      <c r="E371" s="293"/>
-      <c r="F371" s="295"/>
-      <c r="G371" s="293"/>
-      <c r="H371" s="293"/>
-      <c r="I371" s="293"/>
-    </row>
-    <row r="372" spans="1:9">
-      <c r="A372" s="296" t="s">
-        <v>4</v>
-      </c>
-      <c r="B372" s="297" t="s">
-        <v>31</v>
+      <c r="B372" s="292" t="s">
+        <v>211</v>
       </c>
       <c r="C372" s="293"/>
-      <c r="D372" s="293"/>
+      <c r="D372" s="294"/>
       <c r="E372" s="293"/>
       <c r="F372" s="295"/>
       <c r="G372" s="293"/>
@@ -9340,10 +9385,10 @@
     </row>
     <row r="373" spans="1:9">
       <c r="A373" s="296" t="s">
-        <v>5</v>
-      </c>
-      <c r="B373" s="298" t="s">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="B373" s="297">
+        <v>1</v>
       </c>
       <c r="C373" s="293"/>
       <c r="D373" s="293"/>
@@ -9353,396 +9398,208 @@
       <c r="H373" s="293"/>
       <c r="I373" s="293"/>
     </row>
-    <row r="374" spans="1:9" ht="15.75">
-      <c r="A374" s="299" t="s">
+    <row r="374" spans="1:9">
+      <c r="A374" s="296" t="s">
+        <v>3</v>
+      </c>
+      <c r="B374" s="298" t="s">
+        <v>211</v>
+      </c>
+      <c r="C374" s="293"/>
+      <c r="D374" s="293"/>
+      <c r="E374" s="293"/>
+      <c r="F374" s="295"/>
+      <c r="G374" s="293"/>
+      <c r="H374" s="293"/>
+      <c r="I374" s="293"/>
+    </row>
+    <row r="375" spans="1:9">
+      <c r="A375" s="296" t="s">
+        <v>4</v>
+      </c>
+      <c r="B375" s="297" t="s">
+        <v>31</v>
+      </c>
+      <c r="C375" s="293"/>
+      <c r="D375" s="293"/>
+      <c r="E375" s="293"/>
+      <c r="F375" s="295"/>
+      <c r="G375" s="293"/>
+      <c r="H375" s="293"/>
+      <c r="I375" s="293"/>
+    </row>
+    <row r="376" spans="1:9">
+      <c r="A376" s="296" t="s">
+        <v>5</v>
+      </c>
+      <c r="B376" s="298" t="s">
+        <v>5</v>
+      </c>
+      <c r="C376" s="293"/>
+      <c r="D376" s="293"/>
+      <c r="E376" s="293"/>
+      <c r="F376" s="295"/>
+      <c r="G376" s="293"/>
+      <c r="H376" s="293"/>
+      <c r="I376" s="293"/>
+    </row>
+    <row r="377" spans="1:9" ht="15.75">
+      <c r="A377" s="299" t="s">
         <v>6</v>
       </c>
-      <c r="B374" s="292"/>
-      <c r="C374" s="299"/>
-      <c r="D374" s="299"/>
-      <c r="E374" s="299"/>
-      <c r="F374" s="295"/>
-      <c r="G374" s="299"/>
-      <c r="H374" s="299"/>
-      <c r="I374" s="299"/>
-    </row>
-    <row r="375" spans="1:9" ht="15.75">
-      <c r="A375" s="299" t="s">
+      <c r="B377" s="292"/>
+      <c r="C377" s="299"/>
+      <c r="D377" s="299"/>
+      <c r="E377" s="299"/>
+      <c r="F377" s="295"/>
+      <c r="G377" s="299"/>
+      <c r="H377" s="299"/>
+      <c r="I377" s="299"/>
+    </row>
+    <row r="378" spans="1:9" ht="15.75">
+      <c r="A378" s="299" t="s">
         <v>7</v>
       </c>
-      <c r="B375" s="292" t="s">
+      <c r="B378" s="292" t="s">
         <v>8</v>
       </c>
-      <c r="C375" s="299" t="s">
+      <c r="C378" s="299" t="s">
         <v>3</v>
       </c>
-      <c r="D375" s="299" t="s">
+      <c r="D378" s="299" t="s">
         <v>4</v>
       </c>
-      <c r="E375" s="299" t="s">
+      <c r="E378" s="299" t="s">
         <v>5</v>
       </c>
-      <c r="F375" s="300" t="s">
+      <c r="F378" s="300" t="s">
         <v>9</v>
       </c>
-      <c r="G375" s="299" t="s">
+      <c r="G378" s="299" t="s">
         <v>10</v>
       </c>
-      <c r="H375" s="299" t="s">
+      <c r="H378" s="299" t="s">
         <v>11</v>
       </c>
-      <c r="I375" s="299" t="s">
+      <c r="I378" s="299" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="376" spans="1:9">
-      <c r="A376" s="301" t="str">
-        <f>B369</f>
+    <row r="379" spans="1:9">
+      <c r="A379" s="301" t="str">
+        <f>B372</f>
         <v>pill sc2</v>
       </c>
-      <c r="B376" s="302">
-        <f>B370</f>
+      <c r="B379" s="302">
+        <f>B373</f>
         <v>1</v>
       </c>
-      <c r="C376" s="301" t="str">
-        <f>B371</f>
+      <c r="C379" s="301" t="str">
+        <f>B374</f>
         <v>pill sc2</v>
       </c>
-      <c r="D376" s="301" t="str">
-        <f>B372</f>
+      <c r="D379" s="301" t="str">
+        <f>B375</f>
         <v>DK</v>
       </c>
-      <c r="E376" s="301" t="str">
-        <f>B373</f>
+      <c r="E379" s="301" t="str">
+        <f>B376</f>
         <v>unit</v>
       </c>
-      <c r="F376" s="295"/>
-      <c r="G376" s="295" t="s">
+      <c r="F379" s="295"/>
+      <c r="G379" s="295" t="s">
         <v>13</v>
       </c>
-      <c r="H376" s="303" t="str">
+      <c r="H379" s="303" t="str">
         <f>$B$1</f>
         <v>penicillin</v>
       </c>
-      <c r="I376" s="295" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="377" spans="1:9">
-      <c r="A377" s="295" t="s">
+      <c r="I379" s="295" t="s">
         <v>192</v>
       </c>
-      <c r="B377" s="301">
+    </row>
+    <row r="380" spans="1:9">
+      <c r="A380" s="295" t="s">
+        <v>191</v>
+      </c>
+      <c r="B380" s="301">
         <f>5.94*10^-3</f>
         <v>5.9400000000000008E-3</v>
       </c>
-      <c r="C377" s="295" t="s">
+      <c r="C380" s="295" t="s">
         <v>181</v>
       </c>
-      <c r="D377" s="295" t="s">
-        <v>203</v>
-      </c>
-      <c r="E377" s="295" t="s">
-        <v>23</v>
-      </c>
-      <c r="F377" s="295"/>
-      <c r="G377" s="295" t="s">
-        <v>25</v>
-      </c>
-      <c r="H377" s="295" t="s">
-        <v>17</v>
-      </c>
-      <c r="I377" s="295"/>
-    </row>
-    <row r="378" spans="1:9">
-      <c r="A378" s="301" t="str">
+      <c r="D380" s="295" t="s">
+        <v>202</v>
+      </c>
+      <c r="E380" s="295" t="s">
+        <v>23</v>
+      </c>
+      <c r="F380" s="295"/>
+      <c r="G380" s="295" t="s">
+        <v>25</v>
+      </c>
+      <c r="H380" s="295" t="s">
+        <v>17</v>
+      </c>
+      <c r="I380" s="295"/>
+    </row>
+    <row r="381" spans="1:9">
+      <c r="A381" s="301" t="str">
         <f>A211</f>
         <v>packed box of penicillin</v>
       </c>
-      <c r="B378" s="302">
+      <c r="B381" s="302">
         <f>2/3</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="C378" s="301" t="str">
+      <c r="C381" s="301" t="str">
         <f>C211</f>
         <v>box of penicillin</v>
       </c>
-      <c r="D378" s="301" t="str">
-        <f t="shared" ref="D378:E378" si="41">D211</f>
+      <c r="D381" s="301" t="str">
+        <f t="shared" ref="D381:E381" si="41">D211</f>
         <v>SE</v>
       </c>
-      <c r="E378" s="301" t="str">
+      <c r="E381" s="301" t="str">
         <f t="shared" si="41"/>
         <v>unit</v>
       </c>
-      <c r="F378" s="295"/>
-      <c r="G378" s="295" t="s">
-        <v>25</v>
-      </c>
-      <c r="H378" s="301" t="str">
-        <f t="shared" ref="H378" si="42">H211</f>
+      <c r="F381" s="295"/>
+      <c r="G381" s="295" t="s">
+        <v>25</v>
+      </c>
+      <c r="H381" s="301" t="str">
+        <f t="shared" ref="H381" si="42">H211</f>
         <v>penicillin</v>
       </c>
-      <c r="I378" s="295"/>
-    </row>
-    <row r="379" spans="1:9">
-      <c r="A379" s="295" t="s">
+      <c r="I381" s="295"/>
+    </row>
+    <row r="382" spans="1:9">
+      <c r="A382" s="295" t="s">
         <v>160</v>
       </c>
-      <c r="B379" s="301">
+      <c r="B382" s="301">
         <f>-52.64*10^-3</f>
         <v>-5.2639999999999999E-2</v>
       </c>
-      <c r="C379" s="295" t="s">
+      <c r="C382" s="295" t="s">
         <v>159</v>
       </c>
-      <c r="D379" s="295" t="s">
-        <v>203</v>
-      </c>
-      <c r="E379" s="295" t="s">
-        <v>23</v>
-      </c>
-      <c r="F379" s="295"/>
-      <c r="G379" s="295" t="s">
-        <v>25</v>
-      </c>
-      <c r="H379" s="295" t="s">
-        <v>17</v>
-      </c>
-      <c r="I379" s="295"/>
-    </row>
-    <row r="381" spans="1:9" ht="15.75">
-      <c r="A381" s="304" t="s">
-        <v>1</v>
-      </c>
-      <c r="B381" s="305" t="s">
-        <v>213</v>
-      </c>
-      <c r="C381" s="306"/>
-      <c r="D381" s="307"/>
-      <c r="E381" s="306"/>
-      <c r="F381" s="308"/>
-      <c r="G381" s="306"/>
-      <c r="H381" s="306"/>
-      <c r="I381" s="306"/>
-    </row>
-    <row r="382" spans="1:9">
-      <c r="A382" s="309" t="s">
-        <v>2</v>
-      </c>
-      <c r="B382" s="310">
-        <v>1</v>
-      </c>
-      <c r="C382" s="306"/>
-      <c r="D382" s="306"/>
-      <c r="E382" s="306"/>
-      <c r="F382" s="308"/>
-      <c r="G382" s="306"/>
-      <c r="H382" s="306"/>
-      <c r="I382" s="306"/>
-    </row>
-    <row r="383" spans="1:9">
-      <c r="A383" s="309" t="s">
-        <v>3</v>
-      </c>
-      <c r="B383" s="311" t="s">
-        <v>213</v>
-      </c>
-      <c r="C383" s="306"/>
-      <c r="D383" s="306"/>
-      <c r="E383" s="306"/>
-      <c r="F383" s="308"/>
-      <c r="G383" s="306"/>
-      <c r="H383" s="306"/>
-      <c r="I383" s="306"/>
-    </row>
-    <row r="384" spans="1:9">
-      <c r="A384" s="309" t="s">
-        <v>4</v>
-      </c>
-      <c r="B384" s="310" t="s">
-        <v>31</v>
-      </c>
-      <c r="C384" s="306"/>
-      <c r="D384" s="306"/>
-      <c r="E384" s="306"/>
-      <c r="F384" s="308"/>
-      <c r="G384" s="306"/>
-      <c r="H384" s="306"/>
-      <c r="I384" s="306"/>
-    </row>
-    <row r="385" spans="1:9">
-      <c r="A385" s="309" t="s">
-        <v>5</v>
-      </c>
-      <c r="B385" s="311" t="s">
-        <v>5</v>
-      </c>
-      <c r="C385" s="306"/>
-      <c r="D385" s="306"/>
-      <c r="E385" s="306"/>
-      <c r="F385" s="308"/>
-      <c r="G385" s="306"/>
-      <c r="H385" s="306"/>
-      <c r="I385" s="306"/>
-    </row>
-    <row r="386" spans="1:9" ht="15.75">
-      <c r="A386" s="312" t="s">
-        <v>6</v>
-      </c>
-      <c r="B386" s="305"/>
-      <c r="C386" s="312"/>
-      <c r="D386" s="312"/>
-      <c r="E386" s="312"/>
-      <c r="F386" s="308"/>
-      <c r="G386" s="312"/>
-      <c r="H386" s="312"/>
-      <c r="I386" s="312"/>
-    </row>
-    <row r="387" spans="1:9" ht="15.75">
-      <c r="A387" s="312" t="s">
-        <v>7</v>
-      </c>
-      <c r="B387" s="305" t="s">
-        <v>8</v>
-      </c>
-      <c r="C387" s="312" t="s">
-        <v>3</v>
-      </c>
-      <c r="D387" s="312" t="s">
-        <v>4</v>
-      </c>
-      <c r="E387" s="312" t="s">
-        <v>5</v>
-      </c>
-      <c r="F387" s="313" t="s">
-        <v>9</v>
-      </c>
-      <c r="G387" s="312" t="s">
-        <v>10</v>
-      </c>
-      <c r="H387" s="312" t="s">
-        <v>11</v>
-      </c>
-      <c r="I387" s="312" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="388" spans="1:9">
-      <c r="A388" s="314" t="str">
-        <f>B381</f>
-        <v>pill sc3</v>
-      </c>
-      <c r="B388" s="315">
-        <f>B382</f>
-        <v>1</v>
-      </c>
-      <c r="C388" s="314" t="str">
-        <f>B383</f>
-        <v>pill sc3</v>
-      </c>
-      <c r="D388" s="314" t="str">
-        <f>B384</f>
-        <v>DK</v>
-      </c>
-      <c r="E388" s="314" t="str">
-        <f>B385</f>
-        <v>unit</v>
-      </c>
-      <c r="F388" s="308"/>
-      <c r="G388" s="308" t="s">
-        <v>13</v>
-      </c>
-      <c r="H388" s="316" t="str">
-        <f>$B$1</f>
-        <v>penicillin</v>
-      </c>
-      <c r="I388" s="308" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="389" spans="1:9">
-      <c r="A389" s="308" t="s">
-        <v>192</v>
-      </c>
-      <c r="B389" s="314">
-        <f>3.564*10^-3</f>
-        <v>3.5640000000000003E-3</v>
-      </c>
-      <c r="C389" s="308" t="s">
-        <v>181</v>
-      </c>
-      <c r="D389" s="308" t="s">
-        <v>203</v>
-      </c>
-      <c r="E389" s="308" t="s">
-        <v>23</v>
-      </c>
-      <c r="F389" s="308"/>
-      <c r="G389" s="308" t="s">
-        <v>25</v>
-      </c>
-      <c r="H389" s="308" t="s">
-        <v>17</v>
-      </c>
-      <c r="I389" s="308"/>
-    </row>
-    <row r="390" spans="1:9">
-      <c r="A390" s="314" t="str">
-        <f>A211</f>
-        <v>packed box of penicillin</v>
-      </c>
-      <c r="B390" s="315">
-        <f>4/10</f>
-        <v>0.4</v>
-      </c>
-      <c r="C390" s="314" t="str">
-        <f>C211</f>
-        <v>box of penicillin</v>
-      </c>
-      <c r="D390" s="314" t="str">
-        <f t="shared" ref="D390:E390" si="43">D211</f>
-        <v>SE</v>
-      </c>
-      <c r="E390" s="314" t="str">
-        <f t="shared" si="43"/>
-        <v>unit</v>
-      </c>
-      <c r="F390" s="308"/>
-      <c r="G390" s="308" t="s">
-        <v>25</v>
-      </c>
-      <c r="H390" s="314" t="str">
-        <f t="shared" ref="H390" si="44">H211</f>
-        <v>penicillin</v>
-      </c>
-      <c r="I390" s="308"/>
-    </row>
-    <row r="391" spans="1:9">
-      <c r="A391" s="308" t="s">
-        <v>160</v>
-      </c>
-      <c r="B391" s="314">
-        <f>-31.584*10^-3</f>
-        <v>-3.1584000000000001E-2</v>
-      </c>
-      <c r="C391" s="308" t="s">
-        <v>159</v>
-      </c>
-      <c r="D391" s="308" t="s">
-        <v>203</v>
-      </c>
-      <c r="E391" s="308" t="s">
-        <v>23</v>
-      </c>
-      <c r="F391" s="308"/>
-      <c r="G391" s="308" t="s">
-        <v>25</v>
-      </c>
-      <c r="H391" s="308" t="s">
-        <v>17</v>
-      </c>
-      <c r="I391" s="308"/>
+      <c r="D382" s="295" t="s">
+        <v>202</v>
+      </c>
+      <c r="E382" s="295" t="s">
+        <v>23</v>
+      </c>
+      <c r="F382" s="295"/>
+      <c r="G382" s="295" t="s">
+        <v>25</v>
+      </c>
+      <c r="H382" s="295" t="s">
+        <v>17</v>
+      </c>
+      <c r="I382" s="295"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>

</xml_diff>